<commit_message>
Update current consumption calculation for ActivationModule.
</commit_message>
<xml_diff>
--- a/doc/ActivationModule-PowerConsumption.xlsx
+++ b/doc/ActivationModule-PowerConsumption.xlsx
@@ -95,9 +95,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>PWR_DWN; T0,ADC,SPI,WDT,BOD enabled.</t>
-  </si>
-  <si>
     <t>Only output/input, with pullup resistors.</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>Bandgap reading delays 1ms to stabilize measure</t>
+  </si>
+  <si>
+    <t>PWR_DWN; T2,ADC,SPI,WDT,BOD enabled.</t>
   </si>
 </sst>
 </file>
@@ -593,7 +593,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,7 +652,7 @@
         <v>1.5625E-2</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -663,21 +663,21 @@
         <v>500</v>
       </c>
       <c r="C3" s="23">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D3" s="20">
         <v>40</v>
       </c>
       <c r="E3" s="24">
         <f t="shared" ref="E3:E5" si="0">B3/C3/1000</f>
-        <v>1.5625E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="F3" s="25">
         <f t="shared" ref="F3:F6" si="1">D3*E3</f>
-        <v>0.625</v>
+        <v>1.25</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -702,7 +702,7 @@
         <v>1.2E-2</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -710,7 +710,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="15">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="C5" s="4">
         <v>60000</v>
@@ -720,40 +720,35 @@
       </c>
       <c r="E5" s="5">
         <f t="shared" si="0"/>
-        <v>1.6666666666666667E-5</v>
+        <v>3.3333333333333335E-5</v>
       </c>
       <c r="F5" s="17">
         <f t="shared" si="1"/>
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="15">
-        <f>C6*1000*E6</f>
-        <v>31461.666666666664</v>
-      </c>
-      <c r="C6" s="4">
-        <v>32</v>
-      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="13">
         <v>0.36</v>
       </c>
       <c r="E6" s="5">
         <f>1 -SUM(E2:E5)</f>
-        <v>0.98317708333333331</v>
+        <v>0.96753541666666665</v>
       </c>
       <c r="F6" s="17">
         <f t="shared" si="1"/>
-        <v>0.35394375</v>
+        <v>0.34831275</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -778,7 +773,7 @@
       </c>
       <c r="F8" s="18">
         <f>SUM(F2:F6)</f>
-        <v>1.00706875</v>
+        <v>1.62693775</v>
       </c>
       <c r="G8" s="14"/>
     </row>
@@ -804,12 +799,12 @@
         <v>18</v>
       </c>
       <c r="C11" s="3">
-        <f>B11/AVG_CURRENT</f>
-        <v>17.873655596998717</v>
+        <f t="shared" ref="C11:C18" si="2">B11/AVG_CURRENT</f>
+        <v>11.063730004420883</v>
       </c>
       <c r="D11" s="15">
         <f>C11/24</f>
-        <v>0.74473564987494656</v>
+        <v>0.46098875018420343</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -820,12 +815,12 @@
         <v>68</v>
       </c>
       <c r="C12" s="3">
-        <f>B12/AVG_CURRENT</f>
-        <v>67.522698921995143</v>
+        <f t="shared" si="2"/>
+        <v>41.796313350034445</v>
       </c>
       <c r="D12" s="15">
-        <f t="shared" ref="D12:D18" si="2">C12/24</f>
-        <v>2.8134457884164643</v>
+        <f t="shared" ref="D12:D18" si="3">C12/24</f>
+        <v>1.7415130562514352</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -836,12 +831,12 @@
         <v>210</v>
       </c>
       <c r="C13" s="3">
-        <f>B13/AVG_CURRENT</f>
-        <v>208.52598196498502</v>
+        <f t="shared" si="2"/>
+        <v>129.07685005157697</v>
       </c>
       <c r="D13" s="15">
-        <f t="shared" si="2"/>
-        <v>8.6885825818743765</v>
+        <f t="shared" si="3"/>
+        <v>5.378202085482374</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -852,12 +847,12 @@
         <v>900</v>
       </c>
       <c r="C14" s="3">
-        <f>B14/AVG_CURRENT</f>
-        <v>893.68277984993586</v>
+        <f t="shared" si="2"/>
+        <v>553.18650022104407</v>
       </c>
       <c r="D14" s="15">
-        <f t="shared" si="2"/>
-        <v>37.236782493747327</v>
+        <f t="shared" si="3"/>
+        <v>23.049437509210168</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -868,12 +863,12 @@
         <v>1250</v>
       </c>
       <c r="C15" s="3">
-        <f>B15/AVG_CURRENT</f>
-        <v>1241.2260831249109</v>
+        <f t="shared" si="2"/>
+        <v>768.31458364033904</v>
       </c>
       <c r="D15" s="15">
-        <f t="shared" si="2"/>
-        <v>51.717753463537953</v>
+        <f t="shared" si="3"/>
+        <v>32.013107651680791</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -884,12 +879,12 @@
         <v>2400</v>
       </c>
       <c r="C16" s="3">
-        <f>B16/AVG_CURRENT</f>
-        <v>2383.1540795998289</v>
+        <f t="shared" si="2"/>
+        <v>1475.164000589451</v>
       </c>
       <c r="D16" s="15">
-        <f t="shared" si="2"/>
-        <v>99.298086649992868</v>
+        <f t="shared" si="3"/>
+        <v>61.465166691227125</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -900,12 +895,12 @@
         <v>2890</v>
       </c>
       <c r="C17" s="21">
-        <f>B17/AVG_CURRENT</f>
-        <v>2869.7147041847938</v>
+        <f t="shared" si="2"/>
+        <v>1776.3433173764638</v>
       </c>
       <c r="D17" s="22">
-        <f t="shared" si="2"/>
-        <v>119.57144600769975</v>
+        <f t="shared" si="3"/>
+        <v>74.014304890685992</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -916,12 +911,12 @@
         <v>4400</v>
       </c>
       <c r="C18" s="9">
-        <f>B18/AVG_CURRENT</f>
-        <v>4369.1158125996863</v>
+        <f t="shared" si="2"/>
+        <v>2704.4673344139933</v>
       </c>
       <c r="D18" s="16">
-        <f t="shared" si="2"/>
-        <v>182.04649219165358</v>
+        <f t="shared" si="3"/>
+        <v>112.68613893391638</v>
       </c>
     </row>
   </sheetData>

</xml_diff>